<commit_message>
tried KNN and EDA on datasets but AUC has reduced
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Submission</t>
   </si>
@@ -30,8 +30,11 @@
 </t>
   </si>
   <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
     <t>Checking outlliers
-Bivariate and multivariate analysis</t>
+Bivariate and multivariate analysis, KNN, SelectKBest, GridSearchCV</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,8 +468,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>